<commit_message>
Nikon CFI Plan Fluor added
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Detection-obj-overview.xlsx
+++ b/Benchtop/parts-list/Detection-obj-overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BD9342-C247-4970-8FEB-40D0D077C5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E900579-C51A-4587-925E-E9987F781243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8448" yWindow="3636" windowWidth="34560" windowHeight="18684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="100">
   <si>
     <t>Product Name</t>
   </si>
@@ -328,19 +328,32 @@
   </si>
   <si>
     <t>2000 CHF</t>
+  </si>
+  <si>
+    <t>Nikon</t>
+  </si>
+  <si>
+    <t>CFI Plan Fluor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -463,61 +476,62 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3" applyFill="1"/>
-    <xf numFmtId="2" fontId="5" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="5" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -801,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:N40"/>
+  <dimension ref="A3:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42:L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -888,7 +902,7 @@
         <v>7.4000000000000003E-3</v>
       </c>
       <c r="G4" s="14">
-        <f t="shared" ref="G4:G39" si="0">0.5/(2*F4)</f>
+        <f t="shared" ref="G4:G40" si="0">0.5/(2*F4)</f>
         <v>33.783783783783782</v>
       </c>
       <c r="H4" s="2">
@@ -1126,15 +1140,15 @@
         <v>6.0975609756097562</v>
       </c>
       <c r="H10" s="26">
-        <f t="shared" ref="H10:H40" si="16">12.61/A10</f>
+        <f t="shared" ref="H10:H42" si="16">12.61/A10</f>
         <v>25.22</v>
       </c>
       <c r="I10" s="26">
-        <f t="shared" ref="I10:I40" si="17">21.49/A10</f>
+        <f t="shared" ref="I10:I42" si="17">21.49/A10</f>
         <v>42.98</v>
       </c>
       <c r="J10" s="26">
-        <f t="shared" ref="J10:J40" si="18">4.25/A10</f>
+        <f t="shared" ref="J10:J42" si="18">4.25/A10</f>
         <v>8.5</v>
       </c>
       <c r="K10" s="26" t="s">
@@ -2000,84 +2014,86 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="6">
+    <row r="32" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="28">
+        <v>4</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="28">
+        <v>530</v>
+      </c>
+      <c r="E32" s="28">
+        <v>17.2</v>
+      </c>
+      <c r="F32" s="28">
+        <v>0.13</v>
+      </c>
+      <c r="G32" s="30">
+        <v>1.7</v>
+      </c>
+      <c r="H32" s="7">
+        <f t="shared" si="16"/>
+        <v>3.1524999999999999</v>
+      </c>
+      <c r="I32" s="7">
+        <f t="shared" si="17"/>
+        <v>5.3724999999999996</v>
+      </c>
+      <c r="J32" s="7">
+        <f t="shared" si="18"/>
+        <v>1.0625</v>
+      </c>
+      <c r="K32" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="L32" s="36">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="6">
         <v>5</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B33" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C33" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D33" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E33" s="6">
         <v>34</v>
       </c>
-      <c r="F32" s="6">
+      <c r="F33" s="6">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G32" s="13">
+      <c r="G33" s="13">
         <v>2</v>
       </c>
-      <c r="H32" s="7">
+      <c r="H33" s="7">
         <f t="shared" si="16"/>
         <v>2.5219999999999998</v>
       </c>
-      <c r="I32" s="7">
+      <c r="I33" s="7">
         <f t="shared" si="17"/>
         <v>4.298</v>
       </c>
-      <c r="J32" s="7">
+      <c r="J33" s="7">
         <f t="shared" si="18"/>
         <v>0.85</v>
       </c>
-      <c r="K32" s="7" t="s">
+      <c r="K33" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="L32" s="32">
+      <c r="L33" s="32">
         <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>5</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" t="s">
-        <v>77</v>
-      </c>
-      <c r="D33" t="s">
-        <v>66</v>
-      </c>
-      <c r="E33">
-        <v>34</v>
-      </c>
-      <c r="F33">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="G33" s="14">
-        <f t="shared" si="0"/>
-        <v>1.7857142857142856</v>
-      </c>
-      <c r="H33" s="2">
-        <f t="shared" si="16"/>
-        <v>2.5219999999999998</v>
-      </c>
-      <c r="I33" s="2">
-        <f t="shared" si="17"/>
-        <v>4.298</v>
-      </c>
-      <c r="J33" s="2">
-        <f t="shared" si="18"/>
-        <v>0.85</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
@@ -2085,23 +2101,23 @@
         <v>5</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C34" t="s">
         <v>77</v>
       </c>
       <c r="D34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E34">
-        <v>25.5</v>
+        <v>34</v>
       </c>
       <c r="F34">
-        <v>0.21</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G34" s="14">
         <f t="shared" si="0"/>
-        <v>1.1904761904761905</v>
+        <v>1.7857142857142856</v>
       </c>
       <c r="H34" s="2">
         <f t="shared" si="16"/>
@@ -2124,23 +2140,23 @@
         <v>5</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="C35" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="D35" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="E35">
-        <v>18.5</v>
+        <v>25.5</v>
       </c>
       <c r="F35">
-        <v>0.16</v>
+        <v>0.21</v>
       </c>
       <c r="G35" s="14">
         <f t="shared" si="0"/>
-        <v>1.5625</v>
+        <v>1.1904761904761905</v>
       </c>
       <c r="H35" s="2">
         <f t="shared" si="16"/>
@@ -2155,212 +2171,292 @@
         <v>0.85</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="L35" s="33">
-        <v>45</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C36" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D36" t="s">
         <v>25</v>
       </c>
       <c r="E36">
+        <v>18.5</v>
+      </c>
+      <c r="F36">
+        <v>0.16</v>
+      </c>
+      <c r="G36" s="14">
+        <f t="shared" si="0"/>
+        <v>1.5625</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="16"/>
+        <v>2.5219999999999998</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="17"/>
+        <v>4.298</v>
+      </c>
+      <c r="J36" s="2">
+        <f t="shared" si="18"/>
+        <v>0.85</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="L36" s="33">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>6</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" t="s">
         <v>25</v>
       </c>
-      <c r="F36">
+      <c r="E37">
+        <v>25</v>
+      </c>
+      <c r="F37">
         <v>0.3</v>
       </c>
-      <c r="G36" s="14">
+      <c r="G37" s="14">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H36" s="2">
+      <c r="H37" s="2">
         <f t="shared" si="16"/>
         <v>2.1016666666666666</v>
       </c>
-      <c r="I36" s="2">
+      <c r="I37" s="2">
         <f t="shared" si="17"/>
         <v>3.5816666666666666</v>
       </c>
-      <c r="J36" s="2">
+      <c r="J37" s="2">
         <f t="shared" si="18"/>
         <v>0.70833333333333337</v>
       </c>
-      <c r="K36" s="31" t="s">
+      <c r="K37" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="L36" s="36">
+      <c r="L37" s="36">
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="6">
+    <row r="38" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="6">
         <v>7.5</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B38" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C38" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D38" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E38" s="6">
         <v>34</v>
       </c>
-      <c r="F37" s="6">
+      <c r="F38" s="6">
         <v>0.21</v>
       </c>
-      <c r="G37" s="13">
+      <c r="G38" s="13">
         <v>1.3</v>
       </c>
-      <c r="H37" s="7">
+      <c r="H38" s="7">
         <f t="shared" si="16"/>
         <v>1.6813333333333333</v>
       </c>
-      <c r="I37" s="7">
+      <c r="I38" s="7">
         <f t="shared" si="17"/>
         <v>2.8653333333333331</v>
       </c>
-      <c r="J37" s="7">
+      <c r="J38" s="7">
         <f t="shared" si="18"/>
         <v>0.56666666666666665</v>
       </c>
-      <c r="K37" s="7" t="s">
+      <c r="K38" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="L37" s="32">
+      <c r="L38" s="32">
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39">
         <v>7.5</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>77</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>71</v>
       </c>
-      <c r="E38">
+      <c r="E39">
         <v>35</v>
       </c>
-      <c r="F38">
+      <c r="F39">
         <v>0.21</v>
       </c>
-      <c r="G38" s="14">
+      <c r="G39" s="14">
         <f t="shared" si="0"/>
         <v>1.1904761904761905</v>
       </c>
-      <c r="H38" s="2">
+      <c r="H39" s="2">
         <f t="shared" si="16"/>
         <v>1.6813333333333333</v>
       </c>
-      <c r="I38" s="2">
+      <c r="I39" s="2">
         <f t="shared" si="17"/>
         <v>2.8653333333333331</v>
       </c>
-      <c r="J38" s="2">
+      <c r="J39" s="2">
         <f t="shared" si="18"/>
         <v>0.56666666666666665</v>
       </c>
-      <c r="K38" s="2" t="s">
+      <c r="K39" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="6">
+    <row r="40" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="6">
         <v>10</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B40" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C40" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D40" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E40" s="6">
         <v>34</v>
       </c>
-      <c r="F39" s="6">
+      <c r="F40" s="6">
         <v>0.28000000000000003</v>
       </c>
-      <c r="G39" s="13">
+      <c r="G40" s="13">
         <f t="shared" si="0"/>
         <v>0.89285714285714279</v>
       </c>
-      <c r="H39" s="7">
+      <c r="H40" s="7">
         <f t="shared" si="16"/>
         <v>1.2609999999999999</v>
       </c>
-      <c r="I39" s="7">
+      <c r="I40" s="7">
         <f t="shared" si="17"/>
         <v>2.149</v>
       </c>
-      <c r="J39" s="7">
+      <c r="J40" s="7">
         <f t="shared" si="18"/>
         <v>0.42499999999999999</v>
       </c>
-      <c r="K39" s="7" t="s">
+      <c r="K40" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="L39" s="32"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40">
+      <c r="L40" s="32"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41">
         <v>10</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>90</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>87</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>25</v>
       </c>
-      <c r="E40">
+      <c r="E41">
         <v>10</v>
       </c>
-      <c r="F40">
+      <c r="F41">
         <v>0.4</v>
       </c>
-      <c r="G40" s="14">
+      <c r="G41" s="14">
         <v>0.8</v>
       </c>
-      <c r="H40" s="2">
+      <c r="H41" s="2">
         <f t="shared" si="16"/>
         <v>1.2609999999999999</v>
       </c>
-      <c r="I40" s="2">
+      <c r="I41" s="2">
         <f t="shared" si="17"/>
         <v>2.149</v>
       </c>
-      <c r="J40" s="2">
+      <c r="J41" s="2">
         <f t="shared" si="18"/>
         <v>0.42499999999999999</v>
       </c>
-      <c r="K40" s="31" t="s">
+      <c r="K41" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="L40" s="36">
+      <c r="L41" s="36">
         <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" s="6">
+        <v>10</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D42">
+        <v>965</v>
+      </c>
+      <c r="E42" s="6">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="F42" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="G42" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="H42" s="2">
+        <f t="shared" si="16"/>
+        <v>1.2609999999999999</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="17"/>
+        <v>2.149</v>
+      </c>
+      <c r="J42" s="2">
+        <f t="shared" si="18"/>
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="K42" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="L42" s="36">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2381,24 +2477,26 @@
     <hyperlink ref="B23" r:id="rId14" xr:uid="{3E6CF2A1-EE83-4AA4-81AC-316DFC70DCB4}"/>
     <hyperlink ref="B29" r:id="rId15" xr:uid="{83C8F5F9-4F41-4B79-9200-32A2609A2B5A}"/>
     <hyperlink ref="B24" r:id="rId16" display="Plan Apo" xr:uid="{4A338276-1313-4961-8AB0-E02425183408}"/>
-    <hyperlink ref="B32" r:id="rId17" display="Plan Apo" xr:uid="{91EE068A-9052-4609-A361-89B25A613CAB}"/>
-    <hyperlink ref="B37" r:id="rId18" display="Plan Apo" xr:uid="{1DCE0DCD-261B-4BC5-B8A8-7141C7B15F4E}"/>
+    <hyperlink ref="B33" r:id="rId17" display="Plan Apo" xr:uid="{91EE068A-9052-4609-A361-89B25A613CAB}"/>
+    <hyperlink ref="B38" r:id="rId18" display="Plan Apo" xr:uid="{1DCE0DCD-261B-4BC5-B8A8-7141C7B15F4E}"/>
     <hyperlink ref="B25" r:id="rId19" xr:uid="{6E40E3E5-BEB2-4C03-A727-2595EFE56461}"/>
-    <hyperlink ref="B33" r:id="rId20" xr:uid="{7B8B86FD-0E4D-4B40-BE08-5FB6CFC7DD2D}"/>
-    <hyperlink ref="B34" r:id="rId21" display="Plan Apo" xr:uid="{8467164B-0D99-42AE-BE3B-C06EE6572BCC}"/>
-    <hyperlink ref="B38" r:id="rId22" xr:uid="{A49C9EA0-00B2-45B5-B328-8BB20A36800B}"/>
+    <hyperlink ref="B34" r:id="rId20" xr:uid="{7B8B86FD-0E4D-4B40-BE08-5FB6CFC7DD2D}"/>
+    <hyperlink ref="B35" r:id="rId21" display="Plan Apo" xr:uid="{8467164B-0D99-42AE-BE3B-C06EE6572BCC}"/>
+    <hyperlink ref="B39" r:id="rId22" xr:uid="{A49C9EA0-00B2-45B5-B328-8BB20A36800B}"/>
     <hyperlink ref="B16" r:id="rId23" xr:uid="{6702FAF8-6190-4DF2-AC5D-679DF37144DA}"/>
     <hyperlink ref="B9" r:id="rId24" xr:uid="{1AF3E83A-4010-402B-8196-B0C7E8688B12}"/>
-    <hyperlink ref="B39" r:id="rId25" xr:uid="{BC3F733B-619C-42A4-982D-B059501025F8}"/>
+    <hyperlink ref="B40" r:id="rId25" xr:uid="{BC3F733B-619C-42A4-982D-B059501025F8}"/>
     <hyperlink ref="B18" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B17" r:id="rId27" display="1X ICO, 0.04 NA, 15 WD" xr:uid="{15CD43A8-9ABF-44AD-8CA9-4BBDB8853902}"/>
     <hyperlink ref="B26" r:id="rId28" xr:uid="{C61CFBDF-784C-492E-8190-C23C15746450}"/>
     <hyperlink ref="B31" r:id="rId29" display="4X HR Plan Apo" xr:uid="{9B2629BD-CCAC-40F5-BAF4-08E8A93A706B}"/>
-    <hyperlink ref="B36" r:id="rId30" xr:uid="{C8A6F938-3412-4F77-8437-A82E61BCE502}"/>
-    <hyperlink ref="B35" r:id="rId31" xr:uid="{E4CE5BBE-E494-4286-A7C8-209FCE1C79D1}"/>
+    <hyperlink ref="B37" r:id="rId30" xr:uid="{C8A6F938-3412-4F77-8437-A82E61BCE502}"/>
+    <hyperlink ref="B36" r:id="rId31" xr:uid="{E4CE5BBE-E494-4286-A7C8-209FCE1C79D1}"/>
     <hyperlink ref="B27" r:id="rId32" xr:uid="{28FFC81E-134B-417D-9E17-43E8494976AA}"/>
+    <hyperlink ref="B32" r:id="rId33" xr:uid="{BD9602B0-6EB1-4EC3-A257-C17D8B18B8BC}"/>
+    <hyperlink ref="B42" r:id="rId34" xr:uid="{1CB4BA9A-E2FF-47CA-AA4A-0F2AEE5D0BD0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId33"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId35"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mitutoyo Plan Apso are amazing
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Detection-obj-overview.xlsx
+++ b/Benchtop/parts-list/Detection-obj-overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41C3A89-3D3D-4276-B450-FE33C2A8CF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF71F74-E29D-4315-A6C5-031922EE1883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="6828" windowWidth="34560" windowHeight="18684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8352" yWindow="3984" windowWidth="34560" windowHeight="18684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="105">
   <si>
     <t>Product Name</t>
   </si>
@@ -343,6 +343,12 @@
   </si>
   <si>
     <t>M2M32S </t>
+  </si>
+  <si>
+    <t>AMAZING</t>
+  </si>
+  <si>
+    <t>ToDo?</t>
   </si>
 </sst>
 </file>
@@ -826,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1169,7 +1175,7 @@
       <c r="L10" s="34"/>
       <c r="M10" s="25"/>
       <c r="N10" s="25" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -1321,7 +1327,7 @@
       <c r="L14" s="35"/>
       <c r="M14" s="4"/>
       <c r="N14" s="25" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -1738,7 +1744,7 @@
       </c>
       <c r="L24" s="38"/>
       <c r="N24" s="6" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>100</v>
@@ -2079,9 +2085,7 @@
       <c r="L32" s="36">
         <v>60</v>
       </c>
-      <c r="N32" s="6" t="s">
-        <v>97</v>
-      </c>
+      <c r="N32" s="6"/>
     </row>
     <row r="33" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
@@ -2124,7 +2128,7 @@
         <v>95</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="O33" s="1" t="s">
         <v>100</v>
@@ -2332,7 +2336,7 @@
         <v>95</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="O38" s="1" t="s">
         <v>100</v>
@@ -2416,6 +2420,9 @@
         <v>60</v>
       </c>
       <c r="L40" s="32"/>
+      <c r="N40" s="6" t="s">
+        <v>103</v>
+      </c>
       <c r="O40" s="1" t="s">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
update about Leica 1x
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Detection-obj-overview.xlsx
+++ b/Benchtop/parts-list/Detection-obj-overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF71F74-E29D-4315-A6C5-031922EE1883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9341E1C-607F-4D23-B0F5-97E0F597562B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8352" yWindow="3984" windowWidth="34560" windowHeight="18684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8652" yWindow="4272" windowWidth="34560" windowHeight="18684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="106">
   <si>
     <t>Product Name</t>
   </si>
@@ -349,6 +349,9 @@
   </si>
   <si>
     <t>ToDo?</t>
+  </si>
+  <si>
+    <t>Avoid! Strong astigmatism.</t>
   </si>
 </sst>
 </file>
@@ -833,7 +836,7 @@
   <dimension ref="A3:O42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1406,7 +1409,7 @@
       </c>
       <c r="L16" s="32"/>
       <c r="N16" s="6" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
Mitutoyo Plan Apo BD CAD model
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Detection-obj-overview.xlsx
+++ b/Benchtop/parts-list/Detection-obj-overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9341E1C-607F-4D23-B0F5-97E0F597562B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FA9DAE-29D1-43AB-9DB6-C1EB3DE8B735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8652" yWindow="4272" windowWidth="34560" windowHeight="18684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8304" yWindow="3924" windowWidth="34560" windowHeight="18684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -835,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
create mount for 0.9x telecentric lens. Give warning for 0.5x lens due to galvo issues.
</commit_message>
<xml_diff>
--- a/Benchtop/parts-list/Detection-obj-overview.xlsx
+++ b/Benchtop/parts-list/Detection-obj-overview.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop\parts-list\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\GitHub-public\benchtop-hardware\Benchtop\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FA9DAE-29D1-43AB-9DB6-C1EB3DE8B735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8304" yWindow="3924" windowWidth="34560" windowHeight="18684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8310" yWindow="3930" windowWidth="34560" windowHeight="18690"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="109">
   <si>
     <t>Product Name</t>
   </si>
@@ -267,9 +266,6 @@
     <t>Test results using Iris 15, Ronchi ruling, in air and oil</t>
   </si>
   <si>
-    <t>Large size, high cost</t>
-  </si>
-  <si>
     <t>High cost</t>
   </si>
   <si>
@@ -352,13 +348,25 @@
   </si>
   <si>
     <t>Avoid! Strong astigmatism.</t>
+  </si>
+  <si>
+    <t>Galvo scan range too high!</t>
+  </si>
+  <si>
+    <t>Galvos require active cooling</t>
+  </si>
+  <si>
+    <t>Large size, high cost. Galvos require active cooling</t>
+  </si>
+  <si>
+    <t>Identical to BD version</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -452,6 +460,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -533,15 +555,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="3" applyFill="1"/>
-    <xf numFmtId="2" fontId="6" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="6" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -550,6 +569,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -832,31 +854,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.21875" customWidth="1"/>
-    <col min="2" max="2" width="39.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" customWidth="1"/>
-    <col min="5" max="5" width="8.77734375" customWidth="1"/>
-    <col min="6" max="6" width="8.21875" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" style="14" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" style="2"/>
-    <col min="9" max="9" width="11.44140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="7.88671875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="10.21875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="7.33203125" style="33" customWidth="1"/>
-    <col min="13" max="13" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" style="14" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="2"/>
+    <col min="9" max="9" width="11.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="7.28515625" style="31" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>71</v>
       </c>
@@ -885,13 +907,13 @@
         <v>3</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="L3" s="32" t="s">
-        <v>85</v>
+      <c r="L3" s="30" t="s">
+        <v>84</v>
       </c>
       <c r="M3" s="7" t="s">
         <v>31</v>
@@ -900,11 +922,11 @@
         <v>76</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="40">
         <v>0.17899999999999999</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -942,8 +964,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="40">
         <v>0.23799999999999999</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -981,8 +1003,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="40">
         <v>0.28000000000000003</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1020,8 +1042,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="40">
         <v>0.33</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1059,8 +1081,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="40">
         <v>0.35</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1095,8 +1117,8 @@
         <v>12.142857142857144</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="40">
         <v>0.4</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1131,58 +1153,57 @@
         <v>10.625</v>
       </c>
       <c r="K9" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="O9" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="O9" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="25">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="40">
         <v>0.5</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10">
         <v>175</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G10">
         <f t="shared" si="0"/>
         <v>6.0975609756097562</v>
       </c>
-      <c r="H10" s="26">
+      <c r="H10">
         <f t="shared" ref="H10:H42" si="16">12.61/A10</f>
         <v>25.22</v>
       </c>
-      <c r="I10" s="26">
+      <c r="I10">
         <f t="shared" ref="I10:I42" si="17">21.49/A10</f>
         <v>42.98</v>
       </c>
-      <c r="J10" s="26">
+      <c r="J10">
         <f t="shared" ref="J10:J42" si="18">4.25/A10</f>
         <v>8.5</v>
       </c>
-      <c r="K10" s="26" t="s">
+      <c r="K10" t="s">
         <v>46</v>
       </c>
-      <c r="L10" s="34"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="L10"/>
+      <c r="M10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="40">
         <v>0.6</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1217,8 +1238,8 @@
         <v>7.0833333333333339</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="40">
         <v>0.82</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1253,8 +1274,8 @@
         <v>5.1829268292682933</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="41">
         <v>0.92</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1289,7 +1310,7 @@
         <v>4.6195652173913038</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>0.9</v>
       </c>
@@ -1327,13 +1348,15 @@
       <c r="K14" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="L14" s="35"/>
-      <c r="M14" s="4"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="N14" s="25" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1369,7 +1392,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>1</v>
       </c>
@@ -1380,7 +1403,7 @@
         <v>73</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E16" s="6">
         <v>60</v>
@@ -1405,62 +1428,62 @@
         <v>4.25</v>
       </c>
       <c r="K16" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="L16" s="30"/>
+      <c r="N16" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="O16" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="L16" s="32"/>
-      <c r="N16" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="28">
+    </row>
+    <row r="17" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="26">
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="41">
+      <c r="E17" s="38">
         <v>15</v>
       </c>
-      <c r="F17" s="28">
+      <c r="F17" s="26">
         <v>0.04</v>
       </c>
-      <c r="G17" s="30">
+      <c r="G17" s="28">
         <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
-      <c r="H17" s="31">
+      <c r="H17" s="29">
         <f t="shared" si="16"/>
         <v>12.61</v>
       </c>
-      <c r="I17" s="31">
+      <c r="I17" s="29">
         <f t="shared" si="17"/>
         <v>21.49</v>
       </c>
-      <c r="J17" s="31">
+      <c r="J17" s="29">
         <f t="shared" si="18"/>
         <v>4.25</v>
       </c>
-      <c r="K17" s="31" t="s">
+      <c r="K17" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="L17" s="36">
+      <c r="L17" s="33">
         <v>95</v>
       </c>
-      <c r="M17" s="28" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M17" s="26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>1.2</v>
       </c>
@@ -1498,15 +1521,15 @@
       <c r="K18" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="L18" s="35"/>
+      <c r="L18" s="32"/>
       <c r="M18" s="4" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="N18" s="23" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1.3</v>
       </c>
@@ -1542,7 +1565,7 @@
         <v>3.2692307692307692</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1.5</v>
       </c>
@@ -1578,7 +1601,7 @@
         <v>2.8333333333333335</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>2</v>
       </c>
@@ -1620,7 +1643,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>2</v>
       </c>
@@ -1656,14 +1679,14 @@
         <v>2.125</v>
       </c>
       <c r="K22" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="L22" s="37"/>
+        <v>97</v>
+      </c>
+      <c r="L22" s="34"/>
       <c r="M22" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18">
         <v>2</v>
       </c>
@@ -1701,14 +1724,17 @@
       <c r="K23" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="L23" s="38">
+      <c r="L23" s="35">
         <v>95</v>
+      </c>
+      <c r="M23" s="42" t="s">
+        <v>106</v>
       </c>
       <c r="N23" s="23" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18">
         <v>2</v>
       </c>
@@ -1745,15 +1771,18 @@
       <c r="K24" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="L24" s="38"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="42" t="s">
+        <v>106</v>
+      </c>
       <c r="N24" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>2</v>
       </c>
@@ -1773,8 +1802,7 @@
         <v>5.5E-2</v>
       </c>
       <c r="G25" s="16">
-        <f t="shared" si="0"/>
-        <v>4.5454545454545459</v>
+        <v>5</v>
       </c>
       <c r="H25" s="11">
         <f t="shared" si="16"/>
@@ -1791,19 +1819,25 @@
       <c r="K25" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="L25" s="37">
+      <c r="L25" s="34">
         <v>95</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N25" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="O25" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>2</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>25</v>
@@ -1829,22 +1863,22 @@
         <f t="shared" si="18"/>
         <v>2.125</v>
       </c>
-      <c r="K26" s="31" t="s">
+      <c r="K26" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="L26" s="37">
+      <c r="L26" s="34">
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>2.5</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>25</v>
@@ -1870,14 +1904,14 @@
         <f t="shared" si="18"/>
         <v>1.7</v>
       </c>
-      <c r="K27" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="L27" s="37">
+      <c r="K27" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="L27" s="34">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1913,10 +1947,10 @@
         <v>1.4166666666666667</v>
       </c>
       <c r="M28" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>4</v>
       </c>
@@ -1929,7 +1963,7 @@
       <c r="D29" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E29" s="40">
+      <c r="E29" s="37">
         <v>17</v>
       </c>
       <c r="F29" s="6">
@@ -1954,17 +1988,17 @@
       <c r="K29" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="L29" s="32">
+      <c r="L29" s="30">
         <v>60</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N29" s="23" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>4</v>
       </c>
@@ -2002,31 +2036,31 @@
       <c r="K30" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="L30" s="32"/>
+      <c r="L30" s="30"/>
       <c r="N30" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="28">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="26">
         <v>4</v>
       </c>
-      <c r="B31" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="C31" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="D31" s="28" t="s">
+      <c r="B31" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E31" s="28">
+      <c r="E31" s="26">
         <v>20</v>
       </c>
-      <c r="F31" s="28">
+      <c r="F31" s="26">
         <v>0.2</v>
       </c>
-      <c r="G31" s="30">
+      <c r="G31" s="28">
         <v>1.7</v>
       </c>
       <c r="H31" s="7">
@@ -2041,33 +2075,33 @@
         <f t="shared" si="18"/>
         <v>1.0625</v>
       </c>
-      <c r="K31" s="31" t="s">
+      <c r="K31" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="L31" s="36">
+      <c r="L31" s="33">
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="28">
+    <row r="32" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="26">
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="D32" s="28">
+      <c r="C32" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="26">
         <v>530</v>
       </c>
-      <c r="E32" s="28">
+      <c r="E32" s="26">
         <v>17.2</v>
       </c>
-      <c r="F32" s="28">
+      <c r="F32" s="26">
         <v>0.13</v>
       </c>
-      <c r="G32" s="30">
+      <c r="G32" s="28">
         <v>1.7</v>
       </c>
       <c r="H32" s="7">
@@ -2085,12 +2119,12 @@
       <c r="K32" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="L32" s="36">
+      <c r="L32" s="33">
         <v>60</v>
       </c>
       <c r="N32" s="6"/>
     </row>
-    <row r="33" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>5</v>
       </c>
@@ -2127,17 +2161,17 @@
       <c r="K33" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="L33" s="32">
+      <c r="L33" s="30">
         <v>95</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>5</v>
       </c>
@@ -2176,7 +2210,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>5</v>
       </c>
@@ -2215,15 +2249,15 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>5</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D36" t="s">
         <v>25</v>
@@ -2251,21 +2285,21 @@
         <v>0.85</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L36" s="33">
+        <v>91</v>
+      </c>
+      <c r="L36" s="31">
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>6</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C37" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D37" t="s">
         <v>25</v>
@@ -2291,14 +2325,14 @@
         <f t="shared" si="18"/>
         <v>0.70833333333333337</v>
       </c>
-      <c r="K37" s="31" t="s">
+      <c r="K37" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="L37" s="36">
+      <c r="L37" s="33">
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>7.5</v>
       </c>
@@ -2335,17 +2369,17 @@
       <c r="K38" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="L38" s="32">
+      <c r="L38" s="30">
         <v>95</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>7.5</v>
       </c>
@@ -2384,7 +2418,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>10</v>
       </c>
@@ -2395,7 +2429,7 @@
         <v>74</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E40" s="6">
         <v>34</v>
@@ -2422,23 +2456,23 @@
       <c r="K40" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="L40" s="32"/>
+      <c r="L40" s="30"/>
       <c r="N40" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D41" t="s">
         <v>25</v>
@@ -2464,22 +2498,22 @@
         <f t="shared" si="18"/>
         <v>0.42499999999999999</v>
       </c>
-      <c r="K41" s="31" t="s">
+      <c r="K41" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="L41" s="36">
+      <c r="L41" s="33">
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>10</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D42">
         <v>965</v>
@@ -2508,55 +2542,55 @@
       <c r="K42" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="L42" s="36">
+      <c r="L42" s="33">
         <v>60</v>
       </c>
       <c r="N42" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B19" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B15" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B21" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B28" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B5" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B6" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B4" r:id="rId11" display="https://www.edmundoptics.com/p/0179x-35mm-f-mount-titantl-telecentric-lens/38722/" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B10" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B30" r:id="rId13" xr:uid="{9F3CB3DB-A9D8-4F4B-82A3-F2B7FF5C7500}"/>
-    <hyperlink ref="B23" r:id="rId14" xr:uid="{3E6CF2A1-EE83-4AA4-81AC-316DFC70DCB4}"/>
-    <hyperlink ref="B29" r:id="rId15" xr:uid="{83C8F5F9-4F41-4B79-9200-32A2609A2B5A}"/>
-    <hyperlink ref="B24" r:id="rId16" display="Plan Apo" xr:uid="{4A338276-1313-4961-8AB0-E02425183408}"/>
-    <hyperlink ref="B33" r:id="rId17" display="Plan Apo" xr:uid="{91EE068A-9052-4609-A361-89B25A613CAB}"/>
-    <hyperlink ref="B38" r:id="rId18" display="Plan Apo" xr:uid="{1DCE0DCD-261B-4BC5-B8A8-7141C7B15F4E}"/>
-    <hyperlink ref="B25" r:id="rId19" xr:uid="{6E40E3E5-BEB2-4C03-A727-2595EFE56461}"/>
-    <hyperlink ref="B34" r:id="rId20" xr:uid="{7B8B86FD-0E4D-4B40-BE08-5FB6CFC7DD2D}"/>
-    <hyperlink ref="B35" r:id="rId21" display="Plan Apo" xr:uid="{8467164B-0D99-42AE-BE3B-C06EE6572BCC}"/>
-    <hyperlink ref="B39" r:id="rId22" xr:uid="{A49C9EA0-00B2-45B5-B328-8BB20A36800B}"/>
-    <hyperlink ref="B16" r:id="rId23" xr:uid="{6702FAF8-6190-4DF2-AC5D-679DF37144DA}"/>
-    <hyperlink ref="B9" r:id="rId24" xr:uid="{1AF3E83A-4010-402B-8196-B0C7E8688B12}"/>
-    <hyperlink ref="B40" r:id="rId25" xr:uid="{BC3F733B-619C-42A4-982D-B059501025F8}"/>
-    <hyperlink ref="B18" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B17" r:id="rId27" display="1X ICO, 0.04 NA, 15 WD" xr:uid="{15CD43A8-9ABF-44AD-8CA9-4BBDB8853902}"/>
-    <hyperlink ref="B26" r:id="rId28" xr:uid="{C61CFBDF-784C-492E-8190-C23C15746450}"/>
-    <hyperlink ref="B31" r:id="rId29" display="4X HR Plan Apo" xr:uid="{9B2629BD-CCAC-40F5-BAF4-08E8A93A706B}"/>
-    <hyperlink ref="B37" r:id="rId30" xr:uid="{C8A6F938-3412-4F77-8437-A82E61BCE502}"/>
-    <hyperlink ref="B36" r:id="rId31" xr:uid="{E4CE5BBE-E494-4286-A7C8-209FCE1C79D1}"/>
-    <hyperlink ref="B27" r:id="rId32" xr:uid="{28FFC81E-134B-417D-9E17-43E8494976AA}"/>
-    <hyperlink ref="B32" r:id="rId33" xr:uid="{BD9602B0-6EB1-4EC3-A257-C17D8B18B8BC}"/>
-    <hyperlink ref="B42" r:id="rId34" xr:uid="{1CB4BA9A-E2FF-47CA-AA4A-0F2AEE5D0BD0}"/>
-    <hyperlink ref="O33" r:id="rId35" xr:uid="{C65EFFB1-77E5-4ADC-804B-E215BE689FAC}"/>
-    <hyperlink ref="O38" r:id="rId36" xr:uid="{3F8CB11D-1BEA-4188-9A57-C1BC991B672D}"/>
-    <hyperlink ref="O40" r:id="rId37" xr:uid="{8C2230EF-3B7C-4002-A4BB-40D382640BA3}"/>
-    <hyperlink ref="O24" r:id="rId38" xr:uid="{60F0C478-EB01-41BE-931A-F1CC0F19F64D}"/>
-    <hyperlink ref="O16" r:id="rId39" xr:uid="{A6A336D9-F68F-40EB-B5FF-C426C4EE2BE3}"/>
-    <hyperlink ref="O9" r:id="rId40" xr:uid="{F4676AFA-AEBE-4029-8CA3-5991067EACE3}"/>
+    <hyperlink ref="B14" r:id="rId1"/>
+    <hyperlink ref="B19" r:id="rId2"/>
+    <hyperlink ref="B15" r:id="rId3"/>
+    <hyperlink ref="B21" r:id="rId4"/>
+    <hyperlink ref="B28" r:id="rId5"/>
+    <hyperlink ref="B8" r:id="rId6"/>
+    <hyperlink ref="B7" r:id="rId7"/>
+    <hyperlink ref="B5" r:id="rId8"/>
+    <hyperlink ref="B13" r:id="rId9"/>
+    <hyperlink ref="B6" r:id="rId10"/>
+    <hyperlink ref="B4" r:id="rId11" display="https://www.edmundoptics.com/p/0179x-35mm-f-mount-titantl-telecentric-lens/38722/"/>
+    <hyperlink ref="B10" r:id="rId12"/>
+    <hyperlink ref="B30" r:id="rId13"/>
+    <hyperlink ref="B23" r:id="rId14"/>
+    <hyperlink ref="B29" r:id="rId15"/>
+    <hyperlink ref="B24" r:id="rId16" display="Plan Apo"/>
+    <hyperlink ref="B33" r:id="rId17" display="Plan Apo"/>
+    <hyperlink ref="B38" r:id="rId18" display="Plan Apo"/>
+    <hyperlink ref="B25" r:id="rId19"/>
+    <hyperlink ref="B34" r:id="rId20"/>
+    <hyperlink ref="B35" r:id="rId21" display="Plan Apo"/>
+    <hyperlink ref="B39" r:id="rId22"/>
+    <hyperlink ref="B16" r:id="rId23"/>
+    <hyperlink ref="B9" r:id="rId24"/>
+    <hyperlink ref="B40" r:id="rId25"/>
+    <hyperlink ref="B18" r:id="rId26"/>
+    <hyperlink ref="B17" r:id="rId27" display="1X ICO, 0.04 NA, 15 WD"/>
+    <hyperlink ref="B26" r:id="rId28"/>
+    <hyperlink ref="B31" r:id="rId29" display="4X HR Plan Apo"/>
+    <hyperlink ref="B37" r:id="rId30"/>
+    <hyperlink ref="B36" r:id="rId31"/>
+    <hyperlink ref="B27" r:id="rId32"/>
+    <hyperlink ref="B32" r:id="rId33"/>
+    <hyperlink ref="B42" r:id="rId34"/>
+    <hyperlink ref="O33" r:id="rId35"/>
+    <hyperlink ref="O38" r:id="rId36"/>
+    <hyperlink ref="O40" r:id="rId37"/>
+    <hyperlink ref="O24" r:id="rId38"/>
+    <hyperlink ref="O16" r:id="rId39"/>
+    <hyperlink ref="O9" r:id="rId40"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId41"/>

</xml_diff>